<commit_message>
FAC-1248: Minor excel fix
</commit_message>
<xml_diff>
--- a/flickit-assessment-kit/src/test/resources/correct-excel-kit.xlsx
+++ b/flickit-assessment-kit/src/test/resources/correct-excel-kit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MaturityLevels" sheetId="1" state="visible" r:id="rId3"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
   <si>
     <t xml:space="preserve">Cells indicate the percentage of points from the column's maturity level required to reach the maturity level in the row.</t>
   </si>
@@ -185,16 +185,10 @@
     <t xml:space="preserve">Quiz Count</t>
   </si>
   <si>
-    <t xml:space="preserve">DevelopmentCode</t>
-  </si>
-  <si>
     <t xml:space="preserve">Development</t>
   </si>
   <si>
     <t xml:space="preserve">Development Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DevOpsCode</t>
   </si>
   <si>
     <t xml:space="preserve">DevOps</t>
@@ -203,7 +197,7 @@
     <t xml:space="preserve">DevOps Description</t>
   </si>
   <si>
-    <t xml:space="preserve">TeamCollaborationCode</t>
+    <t xml:space="preserve">TeamCollaboration</t>
   </si>
   <si>
     <t xml:space="preserve">Team Collaboration</t>
@@ -321,9 +315,6 @@
   </si>
   <si>
     <t xml:space="preserve">Question TeamCollaboration 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TeamCollaboration</t>
   </si>
   <si>
     <t xml:space="preserve">Q20</t>
@@ -814,7 +805,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1529,7 +1520,7 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -1666,8 +1657,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1697,44 +1688,44 @@
         <v>50</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="D2" s="9" t="n">
         <f aca="false">COUNTIF(Questions!$B:$B, A2)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>55</v>
       </c>
       <c r="D3" s="9" t="n">
         <f aca="false">COUNTIF(Questions!$B:$B, A3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="D4" s="9" t="n">
         <f aca="false">COUNTIF(Questions!$B:$B, A4)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1761,7 +1752,7 @@
   <dimension ref="A1:BE1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -1790,7 +1781,7 @@
       <c r="G1" s="37"/>
       <c r="H1" s="37"/>
       <c r="I1" s="38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J1" s="38"/>
       <c r="K1" s="38"/>
@@ -1812,30 +1803,30 @@
       <c r="AA1" s="39"/>
       <c r="AB1" s="39"/>
     </row>
-    <row r="2" customFormat="false" ht="79.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="D2" s="37" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>63</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="37" t="s">
         <v>64</v>
-      </c>
-      <c r="G2" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>66</v>
       </c>
       <c r="I2" s="41" t="str">
         <f aca="false">IF(QualityAttributes!E2="", "", QualityAttributes!E2)</f>
@@ -1913,19 +1904,19 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="44" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F3" s="44" t="n">
         <v>0</v>
@@ -1958,19 +1949,19 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="43" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" s="44" t="n">
         <v>0</v>
@@ -2003,19 +1994,19 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F5" s="44" t="n">
         <v>1</v>
@@ -2048,19 +2039,19 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D6" s="44" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F6" s="44" t="n">
         <v>0</v>
@@ -2095,19 +2086,19 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="43" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D7" s="44" t="s">
         <v>21</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F7" s="44" t="n">
         <v>1</v>
@@ -27878,7 +27869,7 @@
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
       <c r="D1" s="62" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E1" s="62"/>
       <c r="F1" s="62"/>
@@ -27889,10 +27880,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="63" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2" s="64" t="s">
         <v>49</v>

</xml_diff>